<commit_message>
copy edits and social
</commit_message>
<xml_diff>
--- a/quiz_graphics (2).xlsx
+++ b/quiz_graphics (2).xlsx
@@ -13,9 +13,6 @@
     <sheet name="Q6" sheetId="27" r:id="rId4"/>
     <sheet name="Q10" sheetId="30" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="AdultCost" localSheetId="4">#REF!</definedName>
     <definedName name="AdultCost" localSheetId="2">#REF!</definedName>
@@ -133,15 +130,6 @@
     <t>Top 1 Percent</t>
   </si>
   <si>
-    <t>95-99</t>
-  </si>
-  <si>
-    <t>90-95</t>
-  </si>
-  <si>
-    <t>80-90</t>
-  </si>
-  <si>
     <t>Top Quintile</t>
   </si>
   <si>
@@ -188,6 +176,15 @@
   </si>
   <si>
     <t>Trump                    Married, Childless</t>
+  </si>
+  <si>
+    <t>80–90</t>
+  </si>
+  <si>
+    <t>90–95</t>
+  </si>
+  <si>
+    <t>95–99</t>
   </si>
 </sst>
 </file>
@@ -1533,11 +1530,11 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="1648060600"/>
-        <c:axId val="1648137656"/>
+        <c:axId val="-2061681208"/>
+        <c:axId val="2134521400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1648060600"/>
+        <c:axId val="-2061681208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648137656"/>
+        <c:crossAx val="2134521400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1568,7 +1565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1648137656"/>
+        <c:axId val="2134521400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648060600"/>
+        <c:crossAx val="-2061681208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1733,13 +1730,13 @@
                   <c:v>All</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80-90</c:v>
+                  <c:v>80–90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90-95</c:v>
+                  <c:v>90–95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95-99</c:v>
+                  <c:v>95–99</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Top 1 Percent</c:v>
@@ -1802,11 +1799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="25"/>
-        <c:axId val="1648126040"/>
-        <c:axId val="1648129048"/>
+        <c:axId val="2134173576"/>
+        <c:axId val="2134176632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1648126040"/>
+        <c:axId val="2134173576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1813,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1648129048"/>
+        <c:crossAx val="2134176632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1824,7 +1821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1648129048"/>
+        <c:axId val="2134176632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1850,7 +1847,7 @@
             <a:prstDash val="sysDot"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1648126040"/>
+        <c:crossAx val="2134173576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2106,13 +2103,13 @@
                   <c:v>All</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80-90</c:v>
+                  <c:v>80–90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90-95</c:v>
+                  <c:v>90–95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95-99</c:v>
+                  <c:v>95–99</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Top 1 Percent</c:v>
@@ -2175,11 +2172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="25"/>
-        <c:axId val="1651969928"/>
-        <c:axId val="1651973112"/>
+        <c:axId val="2134592440"/>
+        <c:axId val="2134160824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1651969928"/>
+        <c:axId val="2134592440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +2199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1651973112"/>
+        <c:crossAx val="2134160824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2210,7 +2207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1651973112"/>
+        <c:axId val="2134160824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,7 +2247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1651969928"/>
+        <c:crossAx val="2134592440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2424,11 +2421,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1656443144"/>
-        <c:axId val="1656446568"/>
+        <c:axId val="2133550440"/>
+        <c:axId val="2133553832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1656443144"/>
+        <c:axId val="2133550440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2459,7 +2456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1656446568"/>
+        <c:crossAx val="2133553832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2467,7 +2464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1656446568"/>
+        <c:axId val="2133553832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2E13"/>
@@ -2485,7 +2482,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;$&quot;General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2507,7 +2504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1656443144"/>
+        <c:crossAx val="2133550440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0E12"/>
@@ -2670,13 +2667,13 @@
                   <c:v>All</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80-90</c:v>
+                  <c:v>80–90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90-95</c:v>
+                  <c:v>90–95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95-99</c:v>
+                  <c:v>95–99</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Top 1 Percent</c:v>
@@ -2739,11 +2736,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1501286120"/>
-        <c:axId val="2082648280"/>
+        <c:axId val="2134123624"/>
+        <c:axId val="2134127064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1501286120"/>
+        <c:axId val="2134123624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2770,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082648280"/>
+        <c:crossAx val="2134127064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2781,7 +2778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082648280"/>
+        <c:axId val="2134127064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,7 +2817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501286120"/>
+        <c:crossAx val="2134123624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2995,11 +2992,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1647262392"/>
-        <c:axId val="2082769288"/>
+        <c:axId val="-2131566936"/>
+        <c:axId val="-2131556056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1647262392"/>
+        <c:axId val="-2131566936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3030,7 +3027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082769288"/>
+        <c:crossAx val="-2131556056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3038,7 +3035,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082769288"/>
+        <c:axId val="-2131556056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2E13"/>
@@ -3056,7 +3053,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;$&quot;General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3078,7 +3075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1647262392"/>
+        <c:crossAx val="-2131566936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0E12"/>
@@ -3315,7 +3312,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Avenir Medium"/>
             </a:rPr>
-            <a:t>(Trillions of Dollars)</a:t>
+            <a:t>(Trillions of dollars)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="0" lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
@@ -3713,14 +3710,14 @@
               <a:latin typeface="Avenir Light"/>
               <a:cs typeface="Avenir Light"/>
             </a:rPr>
-            <a:t> deduction, personal exemption and tax rates are from </a:t>
+            <a:t> deduction, personal exemption, and tax rates are from </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000">
               <a:latin typeface="Avenir Light"/>
               <a:cs typeface="Avenir Light"/>
             </a:rPr>
-            <a:t>tax year 2015. In this example, a single filer gets one personal exemptions</a:t>
+            <a:t>tax year 2015. In this example, a single filer gets one personal exemption</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0">
@@ -4218,7 +4215,7 @@
               <a:latin typeface="Avenir Light"/>
               <a:cs typeface="Avenir Light"/>
             </a:rPr>
-            <a:t>Urban-Brookings Tax Policy Center Microsimulation Model (version 0515-3A)</a:t>
+            <a:t>Urban-Brookings Tax Policy Center Microsimulation Model (version 0515-3A).</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4490,7 +4487,27 @@
               <a:ea typeface="Avenir Book" charset="0"/>
               <a:cs typeface="Avenir Book" charset="0"/>
             </a:rPr>
-            <a:t>Trump Plan's, Cumulative Increase in National Debt</a:t>
+            <a:t>Trump</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:effectLst/>
+              <a:latin typeface="Avenir Book"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Avenir Book"/>
+            </a:rPr>
+            <a:t>’</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:rPr>
+            <a:t>s Plan, Cumulative Increase in National Debt</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -4511,7 +4528,7 @@
               <a:ea typeface="Avenir Book" charset="0"/>
               <a:cs typeface="Avenir Book" charset="0"/>
             </a:rPr>
-            <a:t>(Trillions of Dollars)</a:t>
+            <a:t>(Trillions of dollars)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -4750,7 +4767,7 @@
               <a:latin typeface="Avenir Light"/>
               <a:cs typeface="Avenir Light"/>
             </a:rPr>
-            <a:t>Trump's original tax plan as scored by the Tax Policy Center</a:t>
+            <a:t>Trump's original tax plan as scored by the Tax Policy Center.</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5101,75 +5118,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Trump_1. Rates"/>
-      <sheetName val="Trump_2. Revenue"/>
-      <sheetName val="TPC_TABLE"/>
-      <sheetName val="Trump_3. No Income Tax"/>
-      <sheetName val="Trump_4. Distribution"/>
-      <sheetName val="Dist_17"/>
-      <sheetName val="Dist_25"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Current</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="D4">
-            <v>2016</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>Standard Deduction</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Current                           Single</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Trump                              Single</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Current                        Married, Childless</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Trump                             Married, Childless</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="7">
-          <cell r="C7">
-            <v>2017</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:E8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
@@ -5506,8 +5454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5531,7 +5479,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5549,7 +5497,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="B5" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="19">
         <v>25000</v>
@@ -5586,7 +5534,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="22">
         <v>50000</v>
@@ -5603,7 +5551,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="L10" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5617,7 +5565,7 @@
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
       <c r="L11" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5642,7 +5590,7 @@
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="L13" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -5656,7 +5604,7 @@
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="L14" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -6085,8 +6033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6106,7 +6054,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>0.97</v>
@@ -6117,7 +6065,7 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
         <v>3.05</v>
@@ -6128,7 +6076,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>4.9400000000000004</v>
@@ -6139,7 +6087,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
         <v>5.79</v>
@@ -6150,7 +6098,7 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
         <v>9.6999999999999993</v>
@@ -6172,7 +6120,7 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>5.4</v>
@@ -6183,7 +6131,7 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1">
         <v>5.73</v>
@@ -6194,7 +6142,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1">
         <v>8.52</v>
@@ -6736,7 +6684,7 @@
   <dimension ref="A4:Q58"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6796,7 +6744,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>5</v>
@@ -7015,10 +6963,10 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
@@ -7174,10 +7122,10 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>2</v>
@@ -7231,7 +7179,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>5</v>
@@ -7415,10 +7363,10 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
@@ -7568,7 +7516,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>2</v>
@@ -7949,7 +7897,7 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8086,7 +8034,7 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -8112,7 +8060,7 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="9">
         <v>-0.1</v>
@@ -8138,7 +8086,7 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="9">
         <v>-0.1</v>
@@ -8164,7 +8112,7 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="9">
         <v>-0.2</v>
@@ -8190,7 +8138,7 @@
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="9">
         <v>-1.7</v>
@@ -8259,7 +8207,7 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C15" s="9">
         <v>-0.2</v>
@@ -8285,7 +8233,7 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C16" s="9">
         <v>-0.3</v>
@@ -8311,7 +8259,7 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9">
         <v>-0.8</v>
@@ -8572,8 +8520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8633,7 +8581,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>5</v>
@@ -8852,10 +8800,10 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
@@ -9011,13 +8959,13 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>29</v>
       </c>
       <c r="D14" s="23">
         <f t="shared" ref="D14:N14" si="1">D13*1000000000</f>
@@ -9068,7 +9016,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>5</v>
@@ -9252,10 +9200,10 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
@@ -9405,10 +9353,10 @@
     </row>
     <row r="27" spans="1:17">
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" s="23">
         <f t="shared" ref="D27:N27" si="3">D26*1000000000</f>

</xml_diff>